<commit_message>
fix : execl data update
</commit_message>
<xml_diff>
--- a/src/main/resources/data/users.xlsx
+++ b/src/main/resources/data/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26C830CD-39C3-48D8-B9FA-FC0A7E921313}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2596F3D7-A7E8-444A-86FF-AECA24915203}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8856" xr2:uid="{D4CCB1BF-7ED2-4C2E-B4D6-EFD79C7D052F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -104,6 +104,10 @@
   </si>
   <si>
     <t>w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@test.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -150,8 +154,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -468,112 +481,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A0E1F8-3E56-4EFF-BB42-A1493485CE9E}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="L12" sqref="L12:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.296875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="D1" s="3" t="str">
+        <f>A1&amp;B1</f>
+        <v>1@test.com</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="D2" s="3" t="str">
+        <f t="shared" ref="D2:D20" si="0">A2&amp;B2</f>
+        <v>2@test.com</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>3@test.com</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+      <c r="D4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>4@test.com</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="D5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>5@test.com</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+      <c r="D6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>6@test.com</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>7@test.com</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>8@test.com</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>9@test.com</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>10@test.com</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>11@test.com</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>12@test.com</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>13@test.com</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>14@test.com</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>15@test.com</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>16@test.com</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>17@test.com</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>18@test.com</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>19@test.com</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
         <v>19</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>20@test.com</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix : find excel data
</commit_message>
<xml_diff>
--- a/src/main/resources/data/users.xlsx
+++ b/src/main/resources/data/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2596F3D7-A7E8-444A-86FF-AECA24915203}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC4B504-17EF-418A-9BF4-DF3E064D129E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8856" xr2:uid="{D4CCB1BF-7ED2-4C2E-B4D6-EFD79C7D052F}"/>
   </bookViews>
@@ -484,18 +484,18 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12:L13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.296875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -510,7 +510,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -525,7 +525,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -540,7 +540,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -555,7 +555,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -570,7 +570,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -585,7 +585,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -600,7 +600,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -615,7 +615,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -630,7 +630,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -645,7 +645,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -660,7 +660,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -675,7 +675,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -690,7 +690,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -705,7 +705,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -720,7 +720,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -735,7 +735,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -750,7 +750,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -765,7 +765,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -780,7 +780,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">

</xml_diff>